<commit_message>
Adjust screen size and ensure comms are imported
</commit_message>
<xml_diff>
--- a/Scrum Status Form SegFault.xlsx
+++ b/Scrum Status Form SegFault.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duncan.adam18\Documents\final\cis_2017-Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA11D5B-9885-474D-A4E8-C1D6A971443A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234B3762-D6F3-4510-B86A-5DFD01B65958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="70">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -113,15 +113,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>TBA</t>
-  </si>
-  <si>
-    <t>To Be Determined</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Identify major parts of the project</t>
   </si>
   <si>
@@ -225,6 +216,33 @@
   </si>
   <si>
     <t>Design game balance</t>
+  </si>
+  <si>
+    <t>Begin programming</t>
+  </si>
+  <si>
+    <t>Design placeholder sprites</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>~75% Complete</t>
+  </si>
+  <si>
+    <t>POSTPONED TO DEC 5 (Team memeber  MIA)</t>
+  </si>
+  <si>
+    <t>~80% Complete</t>
+  </si>
+  <si>
+    <t>Refine Sprites/Design Backgrounds</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Finish core game concepts/Begin work on sprite rendering</t>
   </si>
 </sst>
 </file>
@@ -741,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -788,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -815,7 +833,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -859,7 +877,7 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -870,7 +888,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
@@ -879,10 +897,10 @@
     <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -957,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA0DA6C-A5EB-451E-A9B2-73656B28F8F2}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1025,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1033,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1052,42 +1070,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1126,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1143,12 +1161,12 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" t="str">
         <f>Cover!C20</f>
@@ -1159,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1195,10 +1213,10 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
@@ -1206,10 +1224,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
@@ -1228,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1296,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1304,7 +1322,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1323,42 +1341,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1398,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1406,16 +1424,15 @@
         <f>'17 Nov'!B32</f>
         <v xml:space="preserve">Jessica </v>
       </c>
-      <c r="C19" t="str">
-        <f>'17 Nov'!C32</f>
-        <v>Create Sprites</v>
+      <c r="C19" t="s">
+        <v>62</v>
       </c>
       <c r="D19">
         <f>'17 Nov'!D32</f>
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1423,16 +1440,15 @@
         <f>'17 Nov'!B33</f>
         <v>Adam/Iszabella</v>
       </c>
-      <c r="C20" t="str">
-        <f>'17 Nov'!C33</f>
-        <v>Complete Programming</v>
+      <c r="C20" t="s">
+        <v>61</v>
       </c>
       <c r="D20">
         <f>'17 Nov'!D33</f>
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1457,44 +1473,44 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
         <v>60</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
       </c>
       <c r="D33" s="1">
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1510,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1578,7 +1594,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1586,7 +1602,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1605,42 +1621,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1658,7 +1674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'28 Nov'!B31</f>
         <v>Jessica</v>
@@ -1679,8 +1695,11 @@
         <f>'28 Nov'!D31</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>'28 Nov'!B32</f>
         <v>Adam</v>
@@ -1693,8 +1712,11 @@
         <f>'28 Nov'!D32</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>'28 Nov'!B33</f>
         <v>Bella</v>
@@ -1707,8 +1729,11 @@
         <f>'28 Nov'!D33</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1742,7 @@
         <v>45265</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1725,37 +1750,46 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1839,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1847,7 +1881,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1866,42 +1900,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1930,43 +1964,43 @@
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'30 Nov'!B31</f>
-        <v>TBA</v>
+        <v>Jessica</v>
       </c>
       <c r="C18" t="str">
         <f>'30 Nov'!C31</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>Refine Sprites/Design Backgrounds</v>
+      </c>
+      <c r="D18" s="1">
         <f>'30 Nov'!D31</f>
-        <v>?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>'30 Nov'!B32</f>
-        <v>TBA</v>
+        <v>Adam</v>
       </c>
       <c r="C19" t="str">
         <f>'30 Nov'!C32</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Finish core game concepts/Begin work on sprite rendering</v>
+      </c>
+      <c r="D19" s="1">
         <f>'30 Nov'!D32</f>
-        <v>?</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>'30 Nov'!B33</f>
-        <v>TBA</v>
+        <v>Bella</v>
       </c>
       <c r="C20" t="str">
         <f>'30 Nov'!C33</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D20" s="1" t="str">
+        <v>Design game balance</v>
+      </c>
+      <c r="D20" s="1">
         <f>'30 Nov'!D33</f>
-        <v>?</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -2059,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2067,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2075,7 +2109,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2094,42 +2128,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2245,7 +2279,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2253,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2261,7 +2295,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2280,42 +2314,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2431,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2439,7 +2473,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2447,7 +2481,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2466,42 +2500,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2546,30 +2580,30 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2658,7 +2692,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -2675,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -2692,7 +2726,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -2749,10 +2783,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -2766,10 +2800,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -2783,10 +2817,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -2800,10 +2834,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -2817,10 +2851,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -3088,7 +3122,7 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>

</xml_diff>

<commit_message>
Finish exe building script
</commit_message>
<xml_diff>
--- a/Scrum Status Form SegFault.xlsx
+++ b/Scrum Status Form SegFault.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duncan.adam18\Documents\final\cis_2017-Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234B3762-D6F3-4510-B86A-5DFD01B65958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E272939A-3414-4306-A3E0-997CF20CCBDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="73">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>Finish core game concepts/Begin work on sprite rendering</t>
+  </si>
+  <si>
+    <t>Finish sprite rendering</t>
+  </si>
+  <si>
+    <t>Finish backgrounds</t>
+  </si>
+  <si>
+    <t>Finish scoring mechanisms</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1803,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,6 +2027,39 @@
       </c>
       <c r="C30" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>